<commit_message>
Added a few edges to the test range edges spreadsheet to get the last few stroke-widths I needed. Completed the centering on the self-referential repressor bars. Cleaned up the code so that it wasn't quite so cluttered.
</commit_message>
<xml_diff>
--- a/test-files/Test_Range_Edge_Sizes.xlsx
+++ b/test-files/Test_Range_Edge_Sizes.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kitsuneh\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-75" yWindow="2805" windowWidth="27660" windowHeight="8580"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="11232"/>
   </bookViews>
   <sheets>
     <sheet name="network_optimized_weights" sheetId="1" r:id="rId1"/>
@@ -125,6 +130,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -173,7 +181,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -208,7 +216,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -420,12 +428,12 @@
   <dimension ref="A1:V22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V23" sqref="V23"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -493,7 +501,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -561,7 +569,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -629,7 +637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -697,7 +705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -765,7 +773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -833,7 +841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -901,7 +909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -924,7 +932,7 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>-0.9</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -969,7 +977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -995,7 +1003,7 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>-0.8</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -1037,7 +1045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1105,7 +1113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1173,7 +1181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1241,7 +1249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1279,7 +1287,7 @@
         <v>0</v>
       </c>
       <c r="M13">
-        <v>0</v>
+        <v>-0.4</v>
       </c>
       <c r="N13">
         <v>0</v>
@@ -1309,7 +1317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1377,7 +1385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1445,7 +1453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1513,7 +1521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1581,7 +1589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1649,7 +1657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1717,7 +1725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1785,7 +1793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1853,7 +1861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1923,5 +1931,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>